<commit_message>
add download option + styling
</commit_message>
<xml_diff>
--- a/server/xlsx/od313.xlsx
+++ b/server/xlsx/od313.xlsx
@@ -947,22 +947,22 @@
         <v>GREECE</v>
       </c>
       <c r="K15" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T15" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W15" t="str">
-        <v>A</v>
+        <v>1</v>
       </c>
       <c r="Z15" t="str">
-        <v>43.25036149</v>
+        <v>43.24756052</v>
       </c>
       <c r="AA15" t="str">
-        <v>-77.63214277</v>
+        <v>-77.62575267</v>
       </c>
       <c r="AB15" t="str">
-        <v>9302-L0089-0447-0030-ED00022</v>
+        <v>9302-L0089-0447-0014-ED00001</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1"/>
@@ -974,22 +974,22 @@
         <v>GREECE</v>
       </c>
       <c r="K17" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T17" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W17" t="str">
-        <v>B</v>
+        <v>10</v>
       </c>
       <c r="Z17" t="str">
-        <v>43.25036859</v>
+        <v>43.25122949</v>
       </c>
       <c r="AA17" t="str">
-        <v>-77.63271995</v>
+        <v>-77.62555477</v>
       </c>
       <c r="AB17" t="str">
-        <v>9302-L0089-0447-0030-ED00024</v>
+        <v>9302-L0089-0447-0014-ED00002</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1"/>
@@ -1001,22 +1001,22 @@
         <v>GREECE</v>
       </c>
       <c r="K19" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T19" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W19" t="str">
-        <v>C</v>
+        <v>11</v>
       </c>
       <c r="Z19" t="str">
-        <v>43.25038195</v>
+        <v>43.25163284</v>
       </c>
       <c r="AA19" t="str">
-        <v>-77.63245235</v>
+        <v>-77.62552175</v>
       </c>
       <c r="AB19" t="str">
-        <v>9302-L0089-0447-0030-ED00025</v>
+        <v>9302-L0089-0447-0014-ED00003</v>
       </c>
     </row>
     <row r="20" ht="12.75" customHeight="1"/>
@@ -1028,22 +1028,22 @@
         <v>GREECE</v>
       </c>
       <c r="K21" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T21" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W21" t="str">
-        <v>D</v>
+        <v>12</v>
       </c>
       <c r="Z21" t="str">
-        <v>43.25059424</v>
+        <v>43.25207443</v>
       </c>
       <c r="AA21" t="str">
-        <v>-77.63245686</v>
+        <v>-77.62551953</v>
       </c>
       <c r="AB21" t="str">
-        <v>9302-L0089-0447-0030-ED00027</v>
+        <v>9302-L0089-0447-0014-ED00004</v>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1"/>
@@ -1055,22 +1055,22 @@
         <v>GREECE</v>
       </c>
       <c r="K23" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T23" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W23" t="str">
-        <v>E</v>
+        <v>12A</v>
       </c>
       <c r="Z23" t="str">
-        <v>43.25098773</v>
+        <v>43.25206079</v>
       </c>
       <c r="AA23" t="str">
-        <v>-77.6324131</v>
+        <v>-77.62539088</v>
       </c>
       <c r="AB23" t="str">
-        <v>9302-L0089-0447-0030-ED00030</v>
+        <v>9302-L0089-0447-0014-ED00005</v>
       </c>
     </row>
     <row r="24" ht="12.75" customHeight="1"/>
@@ -1082,22 +1082,22 @@
         <v>GREECE</v>
       </c>
       <c r="K25" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T25" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W25" t="str">
-        <v>F</v>
+        <v>13</v>
       </c>
       <c r="Z25" t="str">
-        <v>43.2514718</v>
+        <v>43.25241547</v>
       </c>
       <c r="AA25" t="str">
-        <v>-77.6323894</v>
+        <v>-77.62548712</v>
       </c>
       <c r="AB25" t="str">
-        <v>9302-L0089-0447-0030-ED00031</v>
+        <v>9302-L0089-0447-0014-ED00006</v>
       </c>
     </row>
     <row r="26" ht="12.75" customHeight="1"/>
@@ -1109,22 +1109,22 @@
         <v>GREECE</v>
       </c>
       <c r="K27" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T27" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W27" t="str">
-        <v>G</v>
+        <v>2</v>
       </c>
       <c r="Z27" t="str">
-        <v>43.25185455</v>
+        <v>43.247965</v>
       </c>
       <c r="AA27" t="str">
-        <v>-77.63238438</v>
+        <v>-77.62571433</v>
       </c>
       <c r="AB27" t="str">
-        <v>9302-L0089-0447-0030-ED00034</v>
+        <v>9302-L0089-0447-0014-ED00007</v>
       </c>
     </row>
     <row r="28" ht="12.75" customHeight="1"/>
@@ -1136,22 +1136,22 @@
         <v>GREECE</v>
       </c>
       <c r="K29" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T29" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W29" t="str">
-        <v>H</v>
+        <v>3</v>
       </c>
       <c r="Z29" t="str">
-        <v>43.25205448</v>
+        <v>43.24839991</v>
       </c>
       <c r="AA29" t="str">
-        <v>-77.63235686</v>
+        <v>-77.62570716</v>
       </c>
       <c r="AB29" t="str">
-        <v>9302-L0089-0447-0030-ED00035</v>
+        <v>9302-L0089-0447-0014-ED00008</v>
       </c>
     </row>
     <row r="30" ht="12.75" customHeight="1"/>
@@ -1163,22 +1163,22 @@
         <v>GREECE</v>
       </c>
       <c r="K31" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T31" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W31" t="str">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Z31" t="str">
-        <v>43.24225829</v>
+        <v>43.24879487</v>
       </c>
       <c r="AA31" t="str">
-        <v>-77.63361124</v>
+        <v>-77.62569484</v>
       </c>
       <c r="AB31" t="str">
-        <v>9302-L0247-0447-0030-ED00001</v>
+        <v>9302-L0089-0447-0014-ED00009</v>
       </c>
     </row>
     <row r="32" ht="11.65" customHeight="1"/>
@@ -1190,22 +1190,22 @@
         <v>GREECE</v>
       </c>
       <c r="K33" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T33" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W33" t="str">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Z33" t="str">
-        <v>43.242712</v>
+        <v>43.24917954</v>
       </c>
       <c r="AA33" t="str">
-        <v>-77.63360961</v>
+        <v>-77.62566285</v>
       </c>
       <c r="AB33" t="str">
-        <v>9302-L0247-0447-0030-ED00010</v>
+        <v>9302-L0089-0447-0014-ED00012</v>
       </c>
     </row>
     <row r="34"/>
@@ -1217,22 +1217,22 @@
         <v>GREECE</v>
       </c>
       <c r="K35" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T35" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W35" t="str">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z35" t="str">
-        <v>43.24311929</v>
+        <v>43.24960056</v>
       </c>
       <c r="AA35" t="str">
-        <v>-77.63358949</v>
+        <v>-77.62566105</v>
       </c>
       <c r="AB35" t="str">
-        <v>9302-L0247-0447-0030-ED00014</v>
+        <v>9302-L0089-0447-0014-ED00013</v>
       </c>
     </row>
     <row r="36" ht="12.75" customHeight="1"/>
@@ -1244,22 +1244,22 @@
         <v>GREECE</v>
       </c>
       <c r="K37" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T37" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W37" t="str">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z37" t="str">
-        <v>43.2435081</v>
+        <v>43.24995668</v>
       </c>
       <c r="AA37" t="str">
-        <v>-77.63356801</v>
+        <v>-77.62564085</v>
       </c>
       <c r="AB37" t="str">
-        <v>9302-L0247-0447-0030-ED00015</v>
+        <v>9302-L0089-0447-0014-ED00014</v>
       </c>
     </row>
     <row r="38" ht="12.75" customHeight="1"/>
@@ -1271,22 +1271,22 @@
         <v>GREECE</v>
       </c>
       <c r="K39" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T39" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W39" t="str">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Z39" t="str">
-        <v>43.24376009</v>
+        <v>43.25037734</v>
       </c>
       <c r="AA39" t="str">
-        <v>-77.63357139</v>
+        <v>-77.62562927</v>
       </c>
       <c r="AB39" t="str">
-        <v>9302-L0247-0447-0030-ED00016</v>
+        <v>9302-L0089-0447-0014-ED00015</v>
       </c>
     </row>
     <row r="40" ht="12.75" customHeight="1"/>
@@ -1298,22 +1298,22 @@
         <v>GREECE</v>
       </c>
       <c r="K41" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T41" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W41" t="str">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Z41" t="str">
-        <v>43.24419473</v>
+        <v>43.25078659</v>
       </c>
       <c r="AA41" t="str">
-        <v>-77.63355129</v>
+        <v>-77.62556053</v>
       </c>
       <c r="AB41" t="str">
-        <v>9302-L0247-0447-0030-ED00017</v>
+        <v>9302-L0089-0447-0014-ED00016</v>
       </c>
     </row>
     <row r="42" ht="11.65" customHeight="1"/>
@@ -1325,22 +1325,22 @@
         <v>GREECE</v>
       </c>
       <c r="K43" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="T43" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="W43" t="str">
-        <v>7</v>
+        <v>A</v>
       </c>
       <c r="Z43" t="str">
-        <v>43.24445987</v>
+        <v>43.2520973</v>
       </c>
       <c r="AA43" t="str">
-        <v>-77.63355085</v>
+        <v>-77.62471493</v>
       </c>
       <c r="AB43" t="str">
-        <v>9302-L0247-0447-0030-ED00018</v>
+        <v>9302-L0089-0447-0014-ED00017</v>
       </c>
     </row>
     <row r="44"/>
@@ -1963,22 +1963,22 @@
         <v>GREECE</v>
       </c>
       <c r="D6" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G6" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H6" t="str">
-        <v>8</v>
+        <v>A</v>
       </c>
       <c r="I6" t="str">
-        <v>43.24474025</v>
+        <v>43.25206263</v>
       </c>
       <c r="J6" t="str">
-        <v>-77.63354713</v>
+        <v>-77.62600755</v>
       </c>
       <c r="K6" t="str">
-        <v>9302-L0247-0447-0030-ED00019</v>
+        <v>9302-L0089-0447-0014-ED00018</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -1990,22 +1990,22 @@
         <v>GREECE</v>
       </c>
       <c r="D8" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G8" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H8" t="str">
-        <v>9</v>
+        <v>A</v>
       </c>
       <c r="I8" t="str">
-        <v>43.24501423</v>
+        <v>43.24944412</v>
       </c>
       <c r="J8" t="str">
-        <v>-77.63353502</v>
+        <v>-77.62634271</v>
       </c>
       <c r="K8" t="str">
-        <v>9302-L0247-0447-0030-ED00020</v>
+        <v>9302-L0089-0447-0014-ED00019</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -2017,22 +2017,22 @@
         <v>GREECE</v>
       </c>
       <c r="D10" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G10" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H10" t="str">
         <v>A</v>
       </c>
       <c r="I10" t="str">
-        <v>43.24576308</v>
+        <v>43.24706711</v>
       </c>
       <c r="J10" t="str">
-        <v>-77.63399098</v>
+        <v>-77.62649921</v>
       </c>
       <c r="K10" t="str">
-        <v>9302-L0247-0447-0030-ED00021</v>
+        <v>9302-L0089-0447-0014-ED00020</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
@@ -2044,22 +2044,22 @@
         <v>GREECE</v>
       </c>
       <c r="D12" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G12" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H12" t="str">
-        <v>B</v>
+        <v>A1</v>
       </c>
       <c r="I12" t="str">
-        <v>43.24616478</v>
+        <v>43.25229154</v>
       </c>
       <c r="J12" t="str">
-        <v>-77.63398527</v>
+        <v>-77.62597915</v>
       </c>
       <c r="K12" t="str">
-        <v>9302-L0247-0447-0030-ED00023</v>
+        <v>9302-L0089-0447-0014-ED00021</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
@@ -2071,22 +2071,22 @@
         <v>GREECE</v>
       </c>
       <c r="D14" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G14" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H14" t="str">
-        <v>C</v>
+        <v>B</v>
       </c>
       <c r="I14" t="str">
-        <v>43.24656234</v>
+        <v>43.25181293</v>
       </c>
       <c r="J14" t="str">
-        <v>-77.6339654</v>
+        <v>-77.62471801</v>
       </c>
       <c r="K14" t="str">
-        <v>9302-L0247-0447-0030-ED00026</v>
+        <v>9302-L0089-0447-0014-ED00022</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
@@ -2098,22 +2098,22 @@
         <v>GREECE</v>
       </c>
       <c r="D16" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G16" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H16" t="str">
-        <v>D</v>
+        <v>B</v>
       </c>
       <c r="I16" t="str">
-        <v>43.24698104</v>
+        <v>43.24665409</v>
       </c>
       <c r="J16" t="str">
-        <v>-77.63394331</v>
+        <v>-77.62650203</v>
       </c>
       <c r="K16" t="str">
-        <v>9302-L0247-0447-0030-ED00028</v>
+        <v>9302-L0089-0447-0014-ED00023</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
@@ -2125,22 +2125,22 @@
         <v>GREECE</v>
       </c>
       <c r="D18" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G18" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H18" t="str">
-        <v>E</v>
+        <v>B</v>
       </c>
       <c r="I18" t="str">
-        <v>43.247405</v>
+        <v>43.2520106</v>
       </c>
       <c r="J18" t="str">
-        <v>-77.63391674</v>
+        <v>-77.62623312</v>
       </c>
       <c r="K18" t="str">
-        <v>9302-L0247-0447-0030-ED00029</v>
+        <v>9302-L0089-0447-0014-ED00024</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -2152,22 +2152,22 @@
         <v>GREECE</v>
       </c>
       <c r="D20" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G20" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H20" t="str">
-        <v>F</v>
+        <v>B</v>
       </c>
       <c r="I20" t="str">
-        <v>43.24780536</v>
+        <v>43.24904066</v>
       </c>
       <c r="J20" t="str">
-        <v>-77.63390762</v>
+        <v>-77.62636388</v>
       </c>
       <c r="K20" t="str">
-        <v>9302-L0247-0447-0030-ED00032</v>
+        <v>9302-L0089-0447-0014-ED00025</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
@@ -2179,22 +2179,22 @@
         <v>GREECE</v>
       </c>
       <c r="D22" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G22" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H22" t="str">
-        <v>G</v>
+        <v>C</v>
       </c>
       <c r="I22" t="str">
-        <v>43.24820871</v>
+        <v>43.25154578</v>
       </c>
       <c r="J22" t="str">
-        <v>-77.63389496</v>
+        <v>-77.62472368</v>
       </c>
       <c r="K22" t="str">
-        <v>9302-L0247-0447-0030-ED00033</v>
+        <v>9302-L0089-0447-0014-ED00026</v>
       </c>
     </row>
     <row r="23"/>
@@ -2206,22 +2206,22 @@
         <v>GREECE</v>
       </c>
       <c r="D24" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G24" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H24" t="str">
-        <v>H</v>
+        <v>C</v>
       </c>
       <c r="I24" t="str">
-        <v>43.24863384</v>
+        <v>43.24623511</v>
       </c>
       <c r="J24" t="str">
-        <v>-77.63386774</v>
+        <v>-77.62653731</v>
       </c>
       <c r="K24" t="str">
-        <v>9302-L0247-0447-0030-ED00036</v>
+        <v>9302-L0089-0447-0014-ED00027</v>
       </c>
     </row>
     <row r="25"/>
@@ -2233,22 +2233,22 @@
         <v>GREECE</v>
       </c>
       <c r="D26" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G26" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H26" t="str">
-        <v>J</v>
+        <v>C</v>
       </c>
       <c r="I26" t="str">
-        <v>43.24904194</v>
+        <v>43.25166188</v>
       </c>
       <c r="J26" t="str">
-        <v>-77.63385955</v>
+        <v>-77.62624883</v>
       </c>
       <c r="K26" t="str">
-        <v>9302-L0247-0447-0030-ED00037</v>
+        <v>9302-L0089-0447-0014-ED00028</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
@@ -2260,22 +2260,22 @@
         <v>GREECE</v>
       </c>
       <c r="D28" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G28" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H28" t="str">
-        <v>K</v>
+        <v>C</v>
       </c>
       <c r="I28" t="str">
-        <v>43.2494473</v>
+        <v>43.2486476</v>
       </c>
       <c r="J28" t="str">
-        <v>-77.63383783</v>
+        <v>-77.62637868</v>
       </c>
       <c r="K28" t="str">
-        <v>9302-L0247-0447-0030-ED00038</v>
+        <v>9302-L0089-0447-0014-ED00029</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
@@ -2287,22 +2287,22 @@
         <v>GREECE</v>
       </c>
       <c r="D30" t="str">
-        <v>ARMSTRONG RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G30" t="str">
-        <v>329</v>
+        <v>169</v>
       </c>
       <c r="H30" t="str">
-        <v>L</v>
+        <v>D</v>
       </c>
       <c r="I30" t="str">
-        <v>43.24966126</v>
+        <v>43.24821926</v>
       </c>
       <c r="J30" t="str">
-        <v>-77.63380048</v>
+        <v>-77.62641697</v>
       </c>
       <c r="K30" t="str">
-        <v>9302-L0247-0447-0030-ED00039</v>
+        <v>9302-L0089-0447-0014-ED00030</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
@@ -2314,22 +2314,22 @@
         <v>GREECE</v>
       </c>
       <c r="D32" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G32" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H32" t="str">
-        <v>12</v>
+        <v>D</v>
       </c>
       <c r="I32" t="str">
-        <v>43.25036168</v>
+        <v>43.25133134</v>
       </c>
       <c r="J32" t="str">
-        <v>-77.63177493</v>
+        <v>-77.62472961</v>
       </c>
       <c r="K32" t="str">
-        <v>9302-L0089-0447-0070-ED00004</v>
+        <v>9302-L0089-0447-0014-ED00031</v>
       </c>
     </row>
     <row r="33"/>
@@ -2341,22 +2341,22 @@
         <v>GREECE</v>
       </c>
       <c r="D34" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G34" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H34" t="str">
-        <v>11</v>
+        <v>D</v>
       </c>
       <c r="I34" t="str">
-        <v>43.24940519</v>
+        <v>43.25124412</v>
       </c>
       <c r="J34" t="str">
-        <v>-77.63182659</v>
+        <v>-77.62626159</v>
       </c>
       <c r="K34" t="str">
-        <v>9302-L0247-0447-0070-ED00003</v>
+        <v>9302-L0089-0447-0014-ED00032</v>
       </c>
     </row>
     <row r="35"/>
@@ -2368,22 +2368,22 @@
         <v>GREECE</v>
       </c>
       <c r="D36" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G36" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H36" t="str">
-        <v>A</v>
+        <v>E</v>
       </c>
       <c r="I36" t="str">
-        <v>43.24572959</v>
+        <v>43.24782384</v>
       </c>
       <c r="J36" t="str">
-        <v>-77.63268165</v>
+        <v>-77.62645803</v>
       </c>
       <c r="K36" t="str">
-        <v>9302-L0247-0447-0070-ED00017</v>
+        <v>9302-L0089-0447-0014-ED00033</v>
       </c>
     </row>
     <row r="37"/>
@@ -2395,22 +2395,22 @@
         <v>GREECE</v>
       </c>
       <c r="D38" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G38" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H38" t="str">
-        <v>B</v>
+        <v>E</v>
       </c>
       <c r="I38" t="str">
-        <v>43.24591841</v>
+        <v>43.2508259</v>
       </c>
       <c r="J38" t="str">
-        <v>-77.63266817</v>
+        <v>-77.62628717</v>
       </c>
       <c r="K38" t="str">
-        <v>9302-L0247-0447-0070-ED00018</v>
+        <v>9302-L0089-0447-0014-ED00034</v>
       </c>
     </row>
     <row r="39"/>
@@ -2422,22 +2422,22 @@
         <v>GREECE</v>
       </c>
       <c r="D40" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G40" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H40" t="str">
-        <v>C</v>
+        <v>E</v>
       </c>
       <c r="I40" t="str">
-        <v>43.24633213</v>
+        <v>43.25113248</v>
       </c>
       <c r="J40" t="str">
-        <v>-77.63263308</v>
+        <v>-77.62476387</v>
       </c>
       <c r="K40" t="str">
-        <v>9302-L0247-0447-0070-ED00019</v>
+        <v>9302-L0089-0447-0014-ED00035</v>
       </c>
     </row>
     <row r="41"/>
@@ -2449,22 +2449,22 @@
         <v>GREECE</v>
       </c>
       <c r="D42" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G42" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H42" t="str">
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="I42" t="str">
-        <v>43.24672723</v>
+        <v>43.25098006</v>
       </c>
       <c r="J42" t="str">
-        <v>-77.63262647</v>
+        <v>-77.62485538</v>
       </c>
       <c r="K42" t="str">
-        <v>9302-L0247-0447-0070-ED00020</v>
+        <v>9302-L0089-0447-0014-ED00036</v>
       </c>
     </row>
     <row r="43"/>
@@ -2476,22 +2476,22 @@
         <v>GREECE</v>
       </c>
       <c r="D44" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G44" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H44" t="str">
-        <v>E</v>
+        <v>F</v>
       </c>
       <c r="I44" t="str">
-        <v>43.24716135</v>
+        <v>43.24760541</v>
       </c>
       <c r="J44" t="str">
-        <v>-77.63262878</v>
+        <v>-77.62644683</v>
       </c>
       <c r="K44" t="str">
-        <v>9302-L0247-0447-0070-ED00021</v>
+        <v>9302-L0089-0447-0014-ED00037</v>
       </c>
     </row>
     <row r="45"/>
@@ -3119,22 +3119,22 @@
         <v>GREECE</v>
       </c>
       <c r="D6" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G6" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H6" t="str">
         <v>F</v>
       </c>
       <c r="I6" t="str">
-        <v>43.24755135</v>
+        <v>43.25042099</v>
       </c>
       <c r="J6" t="str">
-        <v>-77.6325858</v>
+        <v>-77.62629502</v>
       </c>
       <c r="K6" t="str">
-        <v>9302-L0247-0447-0070-ED00022</v>
+        <v>9302-L0089-0447-0014-ED00038</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -3146,22 +3146,22 @@
         <v>GREECE</v>
       </c>
       <c r="D8" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G8" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H8" t="str">
         <v>G</v>
       </c>
       <c r="I8" t="str">
-        <v>43.24796897</v>
+        <v>43.2500005</v>
       </c>
       <c r="J8" t="str">
-        <v>-77.6325781</v>
+        <v>-77.62632513</v>
       </c>
       <c r="K8" t="str">
-        <v>9302-L0247-0447-0070-ED00023</v>
+        <v>9302-L0089-0447-0014-ED00039</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -3173,22 +3173,22 @@
         <v>GREECE</v>
       </c>
       <c r="D10" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G10" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H10" t="str">
-        <v>G1</v>
+        <v>G</v>
       </c>
       <c r="I10" t="str">
-        <v>43.24785988</v>
+        <v>43.25066037</v>
       </c>
       <c r="J10" t="str">
-        <v>-77.63257241</v>
+        <v>-77.62489455</v>
       </c>
       <c r="K10" t="str">
-        <v>9302-L0247-0447-0070-ED00024</v>
+        <v>9302-L0089-0447-0014-ED00040</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
@@ -3200,22 +3200,22 @@
         <v>GREECE</v>
       </c>
       <c r="D12" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G12" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H12" t="str">
         <v>H</v>
       </c>
       <c r="I12" t="str">
-        <v>43.24837505</v>
+        <v>43.2503428</v>
       </c>
       <c r="J12" t="str">
-        <v>-77.63255257</v>
+        <v>-77.62490795</v>
       </c>
       <c r="K12" t="str">
-        <v>9302-L0247-0447-0070-ED00025</v>
+        <v>9302-L0089-0447-0014-ED00041</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
@@ -3227,22 +3227,22 @@
         <v>GREECE</v>
       </c>
       <c r="D14" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G14" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H14" t="str">
-        <v>J</v>
+        <v>I</v>
       </c>
       <c r="I14" t="str">
-        <v>43.24878905</v>
+        <v>43.2500916</v>
       </c>
       <c r="J14" t="str">
-        <v>-77.63260099</v>
+        <v>-77.62488696</v>
       </c>
       <c r="K14" t="str">
-        <v>9302-L0247-0447-0070-ED00026</v>
+        <v>9302-L0089-0447-0014-ED00042</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
@@ -3254,22 +3254,22 @@
         <v>GREECE</v>
       </c>
       <c r="D16" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G16" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H16" t="str">
-        <v>K</v>
+        <v>J</v>
       </c>
       <c r="I16" t="str">
-        <v>43.24942248</v>
+        <v>43.24992141</v>
       </c>
       <c r="J16" t="str">
-        <v>-77.63276404</v>
+        <v>-77.62489883</v>
       </c>
       <c r="K16" t="str">
-        <v>9302-L0247-0447-0070-ED00027</v>
+        <v>9302-L0089-0447-0014-ED00043</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
@@ -3281,22 +3281,22 @@
         <v>GREECE</v>
       </c>
       <c r="D18" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G18" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H18" t="str">
-        <v>L</v>
+        <v>K</v>
       </c>
       <c r="I18" t="str">
-        <v>43.24941445</v>
+        <v>43.24956055</v>
       </c>
       <c r="J18" t="str">
-        <v>-77.63217786</v>
+        <v>-77.62494489</v>
       </c>
       <c r="K18" t="str">
-        <v>9302-L0247-0447-0070-ED00028</v>
+        <v>9302-L0089-0447-0014-ED00044</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -3308,22 +3308,22 @@
         <v>GREECE</v>
       </c>
       <c r="D20" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G20" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H20" t="str">
-        <v>M</v>
+        <v>L</v>
       </c>
       <c r="I20" t="str">
-        <v>43.24919993</v>
+        <v>43.24927812</v>
       </c>
       <c r="J20" t="str">
-        <v>-77.63251813</v>
+        <v>-77.62493764</v>
       </c>
       <c r="K20" t="str">
-        <v>9302-L0247-0447-0070-ED00029</v>
+        <v>9302-L0089-0447-0014-ED00045</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
@@ -3335,22 +3335,22 @@
         <v>GREECE</v>
       </c>
       <c r="D22" t="str">
-        <v>BISCAYNE DR</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G22" t="str">
-        <v>916</v>
+        <v>169</v>
       </c>
       <c r="H22" t="str">
-        <v>N</v>
+        <v>M</v>
       </c>
       <c r="I22" t="str">
-        <v>43.24940865</v>
+        <v>43.24897592</v>
       </c>
       <c r="J22" t="str">
-        <v>-77.63251207</v>
+        <v>-77.62492055</v>
       </c>
       <c r="K22" t="str">
-        <v>9302-L0247-0447-0070-ED00030</v>
+        <v>9302-L0089-0447-0014-ED00046</v>
       </c>
     </row>
     <row r="23"/>
@@ -3362,22 +3362,22 @@
         <v>GREECE</v>
       </c>
       <c r="D24" t="str">
-        <v>MARWOOD RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G24" t="str">
-        <v>984</v>
+        <v>169</v>
       </c>
       <c r="H24" t="str">
-        <v>A</v>
+        <v>N</v>
       </c>
       <c r="I24" t="str">
-        <v>43.25027232</v>
+        <v>43.2486347</v>
       </c>
       <c r="J24" t="str">
-        <v>-77.63493444</v>
+        <v>-77.62499396</v>
       </c>
       <c r="K24" t="str">
-        <v>9302-L0089-0447-0451-ED00040</v>
+        <v>9302-L0089-0447-0014-ED00047</v>
       </c>
     </row>
     <row r="25"/>
@@ -3389,22 +3389,22 @@
         <v>GREECE</v>
       </c>
       <c r="D26" t="str">
-        <v>MARWOOD RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G26" t="str">
-        <v>984</v>
+        <v>169</v>
       </c>
       <c r="H26" t="str">
-        <v>B</v>
+        <v>O</v>
       </c>
       <c r="I26" t="str">
-        <v>43.25067602</v>
+        <v>43.24822041</v>
       </c>
       <c r="J26" t="str">
-        <v>-77.63491497</v>
+        <v>-77.62497302</v>
       </c>
       <c r="K26" t="str">
-        <v>9302-L0089-0447-0451-ED00044</v>
+        <v>9302-L0089-0447-0014-ED00048</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
@@ -3416,22 +3416,22 @@
         <v>GREECE</v>
       </c>
       <c r="D28" t="str">
-        <v>MARWOOD RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G28" t="str">
-        <v>984</v>
+        <v>169</v>
       </c>
       <c r="H28" t="str">
-        <v>C</v>
+        <v>P</v>
       </c>
       <c r="I28" t="str">
-        <v>43.25108352</v>
+        <v>43.24789705</v>
       </c>
       <c r="J28" t="str">
-        <v>-77.63489482</v>
+        <v>-77.62501799</v>
       </c>
       <c r="K28" t="str">
-        <v>9302-L0089-0447-0451-ED00047</v>
+        <v>9302-L0089-0447-0014-ED00049</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
@@ -3443,22 +3443,22 @@
         <v>GREECE</v>
       </c>
       <c r="D30" t="str">
-        <v>MARWOOD RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G30" t="str">
-        <v>984</v>
+        <v>169</v>
       </c>
       <c r="H30" t="str">
-        <v>D</v>
+        <v>Q</v>
       </c>
       <c r="I30" t="str">
-        <v>43.2514969</v>
+        <v>43.24755056</v>
       </c>
       <c r="J30" t="str">
-        <v>-77.63487094</v>
+        <v>-77.62505289</v>
       </c>
       <c r="K30" t="str">
-        <v>9302-L0089-0447-0451-ED00049</v>
+        <v>9302-L0089-0447-0014-ED00050</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
@@ -3470,22 +3470,22 @@
         <v>GREECE</v>
       </c>
       <c r="D32" t="str">
-        <v>MARWOOD RD</v>
+        <v>ALPINE RD</v>
       </c>
       <c r="G32" t="str">
-        <v>984</v>
+        <v>169</v>
       </c>
       <c r="H32" t="str">
-        <v>E</v>
+        <v>R</v>
       </c>
       <c r="I32" t="str">
-        <v>43.25192764</v>
+        <v>43.24723549</v>
       </c>
       <c r="J32" t="str">
-        <v>-77.63486329</v>
+        <v>-77.62501637</v>
       </c>
       <c r="K32" t="str">
-        <v>9302-L0089-0447-0451-ED00052</v>
+        <v>9302-L0089-0447-0014-ED00051</v>
       </c>
     </row>
     <row r="33"/>
@@ -3497,22 +3497,22 @@
         <v>GREECE</v>
       </c>
       <c r="D34" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G34" t="str">
-        <v>984</v>
+        <v>916</v>
       </c>
       <c r="H34" t="str">
-        <v>F</v>
+        <v>12</v>
       </c>
       <c r="I34" t="str">
-        <v>43.25237169</v>
+        <v>43.25036168</v>
       </c>
       <c r="J34" t="str">
-        <v>-77.63479764</v>
+        <v>-77.63177493</v>
       </c>
       <c r="K34" t="str">
-        <v>9302-L0089-0447-0451-ED00057</v>
+        <v>9302-L0089-0447-0070-ED00004</v>
       </c>
     </row>
     <row r="35"/>
@@ -3524,22 +3524,22 @@
         <v>GREECE</v>
       </c>
       <c r="D36" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G36" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H36" t="str">
-        <v>G</v>
+        <v>11</v>
       </c>
       <c r="I36" t="str">
-        <v>43.25252905</v>
+        <v>43.24940519</v>
       </c>
       <c r="J36" t="str">
-        <v>-77.63481738</v>
+        <v>-77.63182659</v>
       </c>
       <c r="K36" t="str">
-        <v>9302-L0089-0447-0451-ED00060</v>
+        <v>9302-L0247-0447-0070-ED00003</v>
       </c>
     </row>
     <row r="37"/>
@@ -3551,22 +3551,22 @@
         <v>GREECE</v>
       </c>
       <c r="D38" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G38" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H38" t="str">
         <v>A</v>
       </c>
       <c r="I38" t="str">
-        <v>43.25228328</v>
+        <v>43.24572959</v>
       </c>
       <c r="J38" t="str">
-        <v>-77.63371665</v>
+        <v>-77.63268165</v>
       </c>
       <c r="K38" t="str">
-        <v>9302-L0089-0447-0451-ED00070</v>
+        <v>9302-L0247-0447-0070-ED00017</v>
       </c>
     </row>
     <row r="39"/>
@@ -3578,22 +3578,22 @@
         <v>GREECE</v>
       </c>
       <c r="D40" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G40" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H40" t="str">
         <v>B</v>
       </c>
       <c r="I40" t="str">
-        <v>43.25189497</v>
+        <v>43.24591841</v>
       </c>
       <c r="J40" t="str">
-        <v>-77.63375541</v>
+        <v>-77.63266817</v>
       </c>
       <c r="K40" t="str">
-        <v>9302-L0089-0447-0451-ED00071</v>
+        <v>9302-L0247-0447-0070-ED00018</v>
       </c>
     </row>
     <row r="41"/>
@@ -3605,22 +3605,22 @@
         <v>GREECE</v>
       </c>
       <c r="D42" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G42" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H42" t="str">
         <v>C</v>
       </c>
       <c r="I42" t="str">
-        <v>43.25145428</v>
+        <v>43.24633213</v>
       </c>
       <c r="J42" t="str">
-        <v>-77.63376523</v>
+        <v>-77.63263308</v>
       </c>
       <c r="K42" t="str">
-        <v>9302-L0089-0447-0451-ED00072</v>
+        <v>9302-L0247-0447-0070-ED00019</v>
       </c>
     </row>
     <row r="43"/>
@@ -3632,22 +3632,22 @@
         <v>GREECE</v>
       </c>
       <c r="D44" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G44" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H44" t="str">
         <v>D</v>
       </c>
       <c r="I44" t="str">
-        <v>43.25107543</v>
+        <v>43.24672723</v>
       </c>
       <c r="J44" t="str">
-        <v>-77.63377498</v>
+        <v>-77.63262647</v>
       </c>
       <c r="K44" t="str">
-        <v>9302-L0089-0447-0451-ED00073</v>
+        <v>9302-L0247-0447-0070-ED00020</v>
       </c>
     </row>
     <row r="45"/>
@@ -4275,22 +4275,22 @@
         <v>GREECE</v>
       </c>
       <c r="D6" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G6" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H6" t="str">
         <v>E</v>
       </c>
       <c r="I6" t="str">
-        <v>43.25068927</v>
+        <v>43.24716135</v>
       </c>
       <c r="J6" t="str">
-        <v>-77.63372885</v>
+        <v>-77.63262878</v>
       </c>
       <c r="K6" t="str">
-        <v>9302-L0089-0447-0451-ED00074</v>
+        <v>9302-L0247-0447-0070-ED00021</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -4302,22 +4302,22 @@
         <v>GREECE</v>
       </c>
       <c r="D8" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G8" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H8" t="str">
-        <v>G</v>
+        <v>F</v>
       </c>
       <c r="I8" t="str">
-        <v>43.25228297</v>
+        <v>43.24755135</v>
       </c>
       <c r="J8" t="str">
-        <v>-77.63352174</v>
+        <v>-77.6325858</v>
       </c>
       <c r="K8" t="str">
-        <v>9302-L0089-0447-0451-ED00076</v>
+        <v>9302-L0247-0447-0070-ED00022</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -4329,22 +4329,22 @@
         <v>GREECE</v>
       </c>
       <c r="D10" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G10" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H10" t="str">
-        <v>H</v>
+        <v>G</v>
       </c>
       <c r="I10" t="str">
-        <v>43.25227719</v>
+        <v>43.24796897</v>
       </c>
       <c r="J10" t="str">
-        <v>-77.63324667</v>
+        <v>-77.6325781</v>
       </c>
       <c r="K10" t="str">
-        <v>9302-L0089-0447-0451-ED00077</v>
+        <v>9302-L0247-0447-0070-ED00023</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
@@ -4356,22 +4356,22 @@
         <v>GREECE</v>
       </c>
       <c r="D12" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G12" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H12" t="str">
-        <v>1</v>
+        <v>G1</v>
       </c>
       <c r="I12" t="str">
-        <v>43.24202615</v>
+        <v>43.24785988</v>
       </c>
       <c r="J12" t="str">
-        <v>-77.63470942</v>
+        <v>-77.63257241</v>
       </c>
       <c r="K12" t="str">
-        <v>9302-L0247-0447-0451-ED00002</v>
+        <v>9302-L0247-0447-0070-ED00024</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
@@ -4383,22 +4383,22 @@
         <v>GREECE</v>
       </c>
       <c r="D14" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G14" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H14" t="str">
-        <v>10</v>
+        <v>H</v>
       </c>
       <c r="I14" t="str">
-        <v>43.24519388</v>
+        <v>43.24837505</v>
       </c>
       <c r="J14" t="str">
-        <v>-77.63464591</v>
+        <v>-77.63255257</v>
       </c>
       <c r="K14" t="str">
-        <v>9302-L0247-0447-0451-ED00003</v>
+        <v>9302-L0247-0447-0070-ED00025</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
@@ -4410,22 +4410,22 @@
         <v>GREECE</v>
       </c>
       <c r="D16" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G16" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H16" t="str">
-        <v>11</v>
+        <v>J</v>
       </c>
       <c r="I16" t="str">
-        <v>43.24544787</v>
+        <v>43.24878905</v>
       </c>
       <c r="J16" t="str">
-        <v>-77.63467591</v>
+        <v>-77.63260099</v>
       </c>
       <c r="K16" t="str">
-        <v>9302-L0247-0447-0451-ED00004</v>
+        <v>9302-L0247-0447-0070-ED00026</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
@@ -4437,22 +4437,22 @@
         <v>GREECE</v>
       </c>
       <c r="D18" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G18" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H18" t="str">
-        <v>2</v>
+        <v>K</v>
       </c>
       <c r="I18" t="str">
-        <v>43.24244369</v>
+        <v>43.24942248</v>
       </c>
       <c r="J18" t="str">
-        <v>-77.63475082</v>
+        <v>-77.63276404</v>
       </c>
       <c r="K18" t="str">
-        <v>9302-L0247-0447-0451-ED00013</v>
+        <v>9302-L0247-0447-0070-ED00027</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -4464,22 +4464,22 @@
         <v>GREECE</v>
       </c>
       <c r="D20" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G20" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H20" t="str">
-        <v>2A</v>
+        <v>L</v>
       </c>
       <c r="I20" t="str">
-        <v>43.24256291</v>
+        <v>43.24941445</v>
       </c>
       <c r="J20" t="str">
-        <v>-77.63463394</v>
+        <v>-77.63217786</v>
       </c>
       <c r="K20" t="str">
-        <v>9302-L0247-0447-0451-ED00024</v>
+        <v>9302-L0247-0447-0070-ED00028</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
@@ -4491,22 +4491,22 @@
         <v>GREECE</v>
       </c>
       <c r="D22" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G22" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H22" t="str">
-        <v>3</v>
+        <v>M</v>
       </c>
       <c r="I22" t="str">
-        <v>43.24274247</v>
+        <v>43.24919993</v>
       </c>
       <c r="J22" t="str">
-        <v>-77.63474269</v>
+        <v>-77.63251813</v>
       </c>
       <c r="K22" t="str">
-        <v>9302-L0247-0447-0451-ED00025</v>
+        <v>9302-L0247-0447-0070-ED00029</v>
       </c>
     </row>
     <row r="23"/>
@@ -4518,22 +4518,22 @@
         <v>GREECE</v>
       </c>
       <c r="D24" t="str">
-        <v>MARWOOD RD</v>
+        <v>BISCAYNE DR</v>
       </c>
       <c r="G24" t="str">
-        <v>6984</v>
+        <v>916</v>
       </c>
       <c r="H24" t="str">
-        <v>4</v>
+        <v>N</v>
       </c>
       <c r="I24" t="str">
-        <v>43.24301058</v>
+        <v>43.24940865</v>
       </c>
       <c r="J24" t="str">
-        <v>-77.63472087</v>
+        <v>-77.63251207</v>
       </c>
       <c r="K24" t="str">
-        <v>9302-L0247-0447-0451-ED00027</v>
+        <v>9302-L0247-0447-0070-ED00030</v>
       </c>
     </row>
     <row r="25"/>
@@ -4545,22 +4545,22 @@
         <v>GREECE</v>
       </c>
       <c r="D26" t="str">
-        <v>MARWOOD RD</v>
+        <v>GREENLEAF RD</v>
       </c>
       <c r="G26" t="str">
-        <v>6984</v>
+        <v>4608</v>
       </c>
       <c r="H26" t="str">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I26" t="str">
-        <v>43.24326511</v>
+        <v>43.25294659</v>
       </c>
       <c r="J26" t="str">
-        <v>-77.63472221</v>
+        <v>-77.62829745</v>
       </c>
       <c r="K26" t="str">
-        <v>9302-L0247-0447-0451-ED00028</v>
+        <v>9302-L0089-0447-0298-ED00008</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
@@ -4572,22 +4572,22 @@
         <v>GREECE</v>
       </c>
       <c r="D28" t="str">
-        <v>MARWOOD RD</v>
+        <v>GREENLEAF RD</v>
       </c>
       <c r="G28" t="str">
-        <v>6984</v>
+        <v>4608</v>
       </c>
       <c r="H28" t="str">
-        <v>5A</v>
+        <v>3</v>
       </c>
       <c r="I28" t="str">
-        <v>43.2433979</v>
+        <v>43.25353813</v>
       </c>
       <c r="J28" t="str">
-        <v>-77.63461489</v>
+        <v>-77.62826796</v>
       </c>
       <c r="K28" t="str">
-        <v>9302-L0247-0447-0451-ED00029</v>
+        <v>9302-L0089-0447-0298-ED00031</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
@@ -4599,22 +4599,22 @@
         <v>GREECE</v>
       </c>
       <c r="D30" t="str">
-        <v>MARWOOD RD</v>
+        <v>GREENLEAF RD</v>
       </c>
       <c r="G30" t="str">
-        <v>6984</v>
+        <v>4608</v>
       </c>
       <c r="H30" t="str">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I30" t="str">
-        <v>43.24352405</v>
+        <v>43.25328475</v>
       </c>
       <c r="J30" t="str">
-        <v>-77.63469928</v>
+        <v>-77.62825755</v>
       </c>
       <c r="K30" t="str">
-        <v>9302-L0247-0447-0451-ED00030</v>
+        <v>9302-L0089-0447-0298-ED00044</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
@@ -4626,22 +4626,22 @@
         <v>GREECE</v>
       </c>
       <c r="D32" t="str">
-        <v>MARWOOD RD</v>
+        <v>GREENLEAF RD</v>
       </c>
       <c r="G32" t="str">
-        <v>6984</v>
+        <v>4608</v>
       </c>
       <c r="H32" t="str">
-        <v>6A</v>
+        <v>1848.01</v>
       </c>
       <c r="I32" t="str">
-        <v>43.24380685</v>
+        <v>43.25337478</v>
       </c>
       <c r="J32" t="str">
-        <v>-77.63470574</v>
+        <v>-77.62835434</v>
       </c>
       <c r="K32" t="str">
-        <v>9302-L0247-0447-0451-ED00031</v>
+        <v>9302-L0355-0447-0298-MH00101</v>
       </c>
     </row>
     <row r="33"/>
@@ -4653,22 +4653,22 @@
         <v>GREECE</v>
       </c>
       <c r="D34" t="str">
-        <v>MARWOOD RD</v>
+        <v>CLEARVIEW RD</v>
       </c>
       <c r="G34" t="str">
-        <v>6984</v>
+        <v>2144</v>
       </c>
       <c r="H34" t="str">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I34" t="str">
-        <v>43.24408803</v>
+        <v>43.24163412</v>
       </c>
       <c r="J34" t="str">
-        <v>-77.6346869</v>
+        <v>-77.62954065</v>
       </c>
       <c r="K34" t="str">
-        <v>9302-L0247-0447-0451-ED00032</v>
+        <v>9302-L0247-0447-0136-ED00011</v>
       </c>
     </row>
     <row r="35"/>
@@ -4680,22 +4680,22 @@
         <v>GREECE</v>
       </c>
       <c r="D36" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G36" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H36" t="str">
-        <v>7A1</v>
+        <v>11C</v>
       </c>
       <c r="I36" t="str">
-        <v>43.24433648</v>
+        <v>43.24250539</v>
       </c>
       <c r="J36" t="str">
-        <v>-77.63471062</v>
+        <v>-77.64494276</v>
       </c>
       <c r="K36" t="str">
-        <v>9302-L0247-0447-0451-ED00034</v>
+        <v>9302-L0247-0447-0406-ED00005</v>
       </c>
     </row>
     <row r="37"/>
@@ -4707,22 +4707,22 @@
         <v>GREECE</v>
       </c>
       <c r="D38" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G38" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H38" t="str">
-        <v>8</v>
+        <v>11D</v>
       </c>
       <c r="I38" t="str">
-        <v>43.24462389</v>
+        <v>43.24247634</v>
       </c>
       <c r="J38" t="str">
-        <v>-77.63469905</v>
+        <v>-77.64450783</v>
       </c>
       <c r="K38" t="str">
-        <v>9302-L0247-0447-0451-ED00035</v>
+        <v>9302-L0247-0447-0406-ED00006</v>
       </c>
     </row>
     <row r="39"/>
@@ -4734,22 +4734,22 @@
         <v>GREECE</v>
       </c>
       <c r="D40" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G40" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H40" t="str">
-        <v>8A</v>
+        <v>11E</v>
       </c>
       <c r="I40" t="str">
-        <v>43.24446366</v>
+        <v>43.24250994</v>
       </c>
       <c r="J40" t="str">
-        <v>-77.63457756</v>
+        <v>-77.64417309</v>
       </c>
       <c r="K40" t="str">
-        <v>9302-L0247-0447-0451-ED00036</v>
+        <v>9302-L0247-0447-0406-ED00007</v>
       </c>
     </row>
     <row r="41"/>
@@ -4761,22 +4761,22 @@
         <v>GREECE</v>
       </c>
       <c r="D42" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G42" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H42" t="str">
-        <v>9</v>
+        <v>11F</v>
       </c>
       <c r="I42" t="str">
-        <v>43.24491165</v>
+        <v>43.24216425</v>
       </c>
       <c r="J42" t="str">
-        <v>-77.63467095</v>
+        <v>-77.64609089</v>
       </c>
       <c r="K42" t="str">
-        <v>9302-L0247-0447-0451-ED00037</v>
+        <v>9302-L0248-0447-0406-ED00008</v>
       </c>
     </row>
     <row r="43"/>
@@ -4788,22 +4788,22 @@
         <v>GREECE</v>
       </c>
       <c r="D44" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G44" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H44" t="str">
-        <v>A</v>
+        <v>11G</v>
       </c>
       <c r="I44" t="str">
-        <v>43.24325737</v>
+        <v>43.24252223</v>
       </c>
       <c r="J44" t="str">
-        <v>-77.63432933</v>
+        <v>-77.6461087</v>
       </c>
       <c r="K44" t="str">
-        <v>9302-L0247-0447-0451-ED00039</v>
+        <v>9302-L0248-0447-0406-ED00009</v>
       </c>
     </row>
     <row r="45"/>
@@ -5431,22 +5431,22 @@
         <v>GREECE</v>
       </c>
       <c r="D6" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G6" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H6" t="str">
-        <v>A</v>
+        <v>1</v>
       </c>
       <c r="I6" t="str">
-        <v>43.24580796</v>
+        <v>43.2439159</v>
       </c>
       <c r="J6" t="str">
-        <v>-77.63513137</v>
+        <v>-77.64663618</v>
       </c>
       <c r="K6" t="str">
-        <v>9302-L0247-0447-0451-ED00041</v>
+        <v>9302-L0250-0447-0406-ED00001</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -5458,22 +5458,22 @@
         <v>GREECE</v>
       </c>
       <c r="D8" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G8" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H8" t="str">
-        <v>A</v>
+        <v>11A</v>
       </c>
       <c r="I8" t="str">
-        <v>43.24256017</v>
+        <v>43.24355134</v>
       </c>
       <c r="J8" t="str">
-        <v>-77.63527831</v>
+        <v>-77.64614036</v>
       </c>
       <c r="K8" t="str">
-        <v>9302-L0247-0447-0451-ED00042</v>
+        <v>9302-L0250-0447-0406-ED00003</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -5485,22 +5485,22 @@
         <v>GREECE</v>
       </c>
       <c r="D10" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G10" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H10" t="str">
-        <v>B</v>
+        <v>11B</v>
       </c>
       <c r="I10" t="str">
-        <v>43.24296357</v>
+        <v>43.24309891</v>
       </c>
       <c r="J10" t="str">
-        <v>-77.63521319</v>
+        <v>-77.64614836</v>
       </c>
       <c r="K10" t="str">
-        <v>9302-L0247-0447-0451-ED00043</v>
+        <v>9302-L0250-0447-0406-ED00004</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
@@ -5512,22 +5512,22 @@
         <v>GREECE</v>
       </c>
       <c r="D12" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G12" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H12" t="str">
-        <v>B</v>
+        <v>11H</v>
       </c>
       <c r="I12" t="str">
-        <v>43.24618516</v>
+        <v>43.24328515</v>
       </c>
       <c r="J12" t="str">
-        <v>-77.63510529</v>
+        <v>-77.64504899</v>
       </c>
       <c r="K12" t="str">
-        <v>9302-L0247-0447-0451-ED00045</v>
+        <v>9302-L0250-0447-0406-ED00010</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
@@ -5539,22 +5539,22 @@
         <v>GREECE</v>
       </c>
       <c r="D14" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G14" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H14" t="str">
-        <v>C</v>
+        <v>11J</v>
       </c>
       <c r="I14" t="str">
-        <v>43.24656826</v>
+        <v>43.24333866</v>
       </c>
       <c r="J14" t="str">
-        <v>-77.63509446</v>
+        <v>-77.64443704</v>
       </c>
       <c r="K14" t="str">
-        <v>9302-L0247-0447-0451-ED00046</v>
+        <v>9302-L0250-0447-0406-ED00011</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
@@ -5566,22 +5566,22 @@
         <v>GREECE</v>
       </c>
       <c r="D16" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G16" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H16" t="str">
-        <v>C</v>
+        <v>11K</v>
       </c>
       <c r="I16" t="str">
-        <v>43.24329514</v>
+        <v>43.24335649</v>
       </c>
       <c r="J16" t="str">
-        <v>-77.63520648</v>
+        <v>-77.64416206</v>
       </c>
       <c r="K16" t="str">
-        <v>9302-L0247-0447-0451-ED00048</v>
+        <v>9302-L0250-0447-0406-ED00012</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
@@ -5593,22 +5593,22 @@
         <v>GREECE</v>
       </c>
       <c r="D18" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G18" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H18" t="str">
-        <v>D</v>
+        <v>11L</v>
       </c>
       <c r="I18" t="str">
-        <v>43.24695276</v>
+        <v>43.24352172</v>
       </c>
       <c r="J18" t="str">
-        <v>-77.63506487</v>
+        <v>-77.6436245</v>
       </c>
       <c r="K18" t="str">
-        <v>9302-L0247-0447-0451-ED00050</v>
+        <v>9302-L0250-0447-0406-ED00013</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
@@ -5620,22 +5620,22 @@
         <v>GREECE</v>
       </c>
       <c r="D20" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G20" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H20" t="str">
-        <v>D</v>
+        <v>11M1</v>
       </c>
       <c r="I20" t="str">
-        <v>43.24369599</v>
+        <v>43.24368718</v>
       </c>
       <c r="J20" t="str">
-        <v>-77.63522237</v>
+        <v>-77.64286205</v>
       </c>
       <c r="K20" t="str">
-        <v>9302-L0247-0447-0451-ED00051</v>
+        <v>9302-L0250-0447-0406-ED00014</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
@@ -5647,22 +5647,22 @@
         <v>GREECE</v>
       </c>
       <c r="D22" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G22" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H22" t="str">
-        <v>E</v>
+        <v>11N</v>
       </c>
       <c r="I22" t="str">
-        <v>43.24733955</v>
+        <v>43.24398278</v>
       </c>
       <c r="J22" t="str">
-        <v>-77.63506147</v>
+        <v>-77.64267074</v>
       </c>
       <c r="K22" t="str">
-        <v>9302-L0247-0447-0451-ED00053</v>
+        <v>9302-L0250-0447-0406-ED00015</v>
       </c>
     </row>
     <row r="23"/>
@@ -5674,22 +5674,22 @@
         <v>GREECE</v>
       </c>
       <c r="D24" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G24" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H24" t="str">
-        <v>E</v>
+        <v>11O</v>
       </c>
       <c r="I24" t="str">
-        <v>43.24407499</v>
+        <v>43.24421886</v>
       </c>
       <c r="J24" t="str">
-        <v>-77.63525008</v>
+        <v>-77.6423789</v>
       </c>
       <c r="K24" t="str">
-        <v>9302-L0247-0447-0451-ED00054</v>
+        <v>9302-L0250-0447-0406-ED00016</v>
       </c>
     </row>
     <row r="25"/>
@@ -5701,22 +5701,22 @@
         <v>GREECE</v>
       </c>
       <c r="D26" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G26" t="str">
-        <v>6984</v>
+        <v>192</v>
       </c>
       <c r="H26" t="str">
-        <v>E1</v>
+        <v>11P</v>
       </c>
       <c r="I26" t="str">
-        <v>43.24744841</v>
+        <v>43.24456409</v>
       </c>
       <c r="J26" t="str">
-        <v>-77.63505878</v>
+        <v>-77.6419979</v>
       </c>
       <c r="K26" t="str">
-        <v>9302-L0247-0447-0451-ED00055</v>
+        <v>9302-L0250-0447-0406-ED00017</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
@@ -5728,22 +5728,22 @@
         <v>GREECE</v>
       </c>
       <c r="D28" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G28" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H28" t="str">
-        <v>F</v>
+        <v>11Q</v>
       </c>
       <c r="I28" t="str">
-        <v>43.24442625</v>
+        <v>43.2447372</v>
       </c>
       <c r="J28" t="str">
-        <v>-77.6352191</v>
+        <v>-77.64181454</v>
       </c>
       <c r="K28" t="str">
-        <v>9302-L0247-0447-0451-ED00056</v>
+        <v>9302-L0250-0447-0406-ED00018</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
@@ -5755,22 +5755,22 @@
         <v>GREECE</v>
       </c>
       <c r="D30" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G30" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H30" t="str">
-        <v>F</v>
+        <v>11R</v>
       </c>
       <c r="I30" t="str">
-        <v>43.24771554</v>
+        <v>43.24404953</v>
       </c>
       <c r="J30" t="str">
-        <v>-77.63504007</v>
+        <v>-77.64227728</v>
       </c>
       <c r="K30" t="str">
-        <v>9302-L0247-0447-0451-ED00058</v>
+        <v>9302-L0250-0447-0406-ED00019</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
@@ -5782,22 +5782,22 @@
         <v>GREECE</v>
       </c>
       <c r="D32" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G32" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H32" t="str">
-        <v>F1</v>
+        <v>11S</v>
       </c>
       <c r="I32" t="str">
-        <v>43.24789717</v>
+        <v>43.24360381</v>
       </c>
       <c r="J32" t="str">
-        <v>-77.63506432</v>
+        <v>-77.64227764</v>
       </c>
       <c r="K32" t="str">
-        <v>9302-L0247-0447-0451-ED00059</v>
+        <v>9302-L0250-0447-0406-ED00020</v>
       </c>
     </row>
     <row r="33"/>
@@ -5809,22 +5809,22 @@
         <v>GREECE</v>
       </c>
       <c r="D34" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G34" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H34" t="str">
-        <v>G</v>
+        <v>11T</v>
       </c>
       <c r="I34" t="str">
-        <v>43.24811056</v>
+        <v>43.24312364</v>
       </c>
       <c r="J34" t="str">
-        <v>-77.63500919</v>
+        <v>-77.64408081</v>
       </c>
       <c r="K34" t="str">
-        <v>9302-L0247-0447-0451-ED00061</v>
+        <v>9302-L0250-0447-0406-ED00021</v>
       </c>
     </row>
     <row r="35"/>
@@ -5836,22 +5836,22 @@
         <v>GREECE</v>
       </c>
       <c r="D36" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G36" t="str">
-        <v>984</v>
+        <v>192</v>
       </c>
       <c r="H36" t="str">
-        <v>G</v>
+        <v>11U</v>
       </c>
       <c r="I36" t="str">
-        <v>43.2448554</v>
+        <v>43.24290411</v>
       </c>
       <c r="J36" t="str">
-        <v>-77.63519006</v>
+        <v>-77.64424673</v>
       </c>
       <c r="K36" t="str">
-        <v>9302-L0247-0447-0451-ED00062</v>
+        <v>9302-L0250-0447-0406-ED00022</v>
       </c>
     </row>
     <row r="37"/>
@@ -5863,22 +5863,22 @@
         <v>GREECE</v>
       </c>
       <c r="D38" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G38" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H38" t="str">
-        <v>H</v>
+        <v>11V</v>
       </c>
       <c r="I38" t="str">
-        <v>43.24524825</v>
+        <v>43.24327431</v>
       </c>
       <c r="J38" t="str">
-        <v>-77.63521433</v>
+        <v>-77.6453732</v>
       </c>
       <c r="K38" t="str">
-        <v>9302-L0247-0447-0451-ED00063</v>
+        <v>9302-L0250-0447-0406-ED00023</v>
       </c>
     </row>
     <row r="39"/>
@@ -5890,22 +5890,22 @@
         <v>GREECE</v>
       </c>
       <c r="D40" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G40" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H40" t="str">
-        <v>H</v>
+        <v>2</v>
       </c>
       <c r="I40" t="str">
-        <v>43.24847053</v>
+        <v>43.24390094</v>
       </c>
       <c r="J40" t="str">
-        <v>-77.63502665</v>
+        <v>-77.64613418</v>
       </c>
       <c r="K40" t="str">
-        <v>9302-L0247-0447-0451-ED00064</v>
+        <v>9302-L0250-0447-0406-ED00024</v>
       </c>
     </row>
     <row r="41"/>
@@ -5917,22 +5917,22 @@
         <v>GREECE</v>
       </c>
       <c r="D42" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G42" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H42" t="str">
-        <v>J</v>
+        <v>3</v>
       </c>
       <c r="I42" t="str">
-        <v>43.24887496</v>
+        <v>43.2439094</v>
       </c>
       <c r="J42" t="str">
-        <v>-77.63497104</v>
+        <v>-77.64542462</v>
       </c>
       <c r="K42" t="str">
-        <v>9302-L0247-0447-0451-ED00065</v>
+        <v>9302-L0250-0447-0406-ED00025</v>
       </c>
     </row>
     <row r="43"/>
@@ -5944,22 +5944,22 @@
         <v>GREECE</v>
       </c>
       <c r="D44" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G44" t="str">
-        <v>6984</v>
+        <v>6192</v>
       </c>
       <c r="H44" t="str">
-        <v>K</v>
+        <v>4</v>
       </c>
       <c r="I44" t="str">
-        <v>43.24931567</v>
+        <v>43.24389429</v>
       </c>
       <c r="J44" t="str">
-        <v>-77.63497935</v>
+        <v>-77.64493783</v>
       </c>
       <c r="K44" t="str">
-        <v>9302-L0247-0447-0451-ED00066</v>
+        <v>9302-L0250-0447-0406-ED00026</v>
       </c>
     </row>
     <row r="45"/>
@@ -6587,22 +6587,22 @@
         <v>GREECE</v>
       </c>
       <c r="D6" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G6" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H6" t="str">
-        <v>L</v>
+        <v>11M</v>
       </c>
       <c r="I6" t="str">
-        <v>43.24956752</v>
+        <v>43.24375654</v>
       </c>
       <c r="J6" t="str">
-        <v>-77.63498204</v>
+        <v>-77.64315943</v>
       </c>
       <c r="K6" t="str">
-        <v>9302-L0247-0447-0451-ED00067</v>
+        <v>9302-L0250-0447-0406-ED00032</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
@@ -6614,22 +6614,22 @@
         <v>GREECE</v>
       </c>
       <c r="D8" t="str">
-        <v>MARWOOD RD</v>
+        <v>LAWSON RD</v>
       </c>
       <c r="G8" t="str">
-        <v>984</v>
+        <v>6192</v>
       </c>
       <c r="H8" t="str">
-        <v>M</v>
+        <v>2140.06</v>
       </c>
       <c r="I8" t="str">
-        <v>43.2478697</v>
+        <v>43.24387458</v>
       </c>
       <c r="J8" t="str">
-        <v>-77.63548435</v>
+        <v>-77.64502817</v>
       </c>
       <c r="K8" t="str">
-        <v>9302-L0247-0447-0451-ED00068</v>
+        <v>9302-L0250-0447-0406-HH00001</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
@@ -6637,485 +6637,107 @@
       <c r="A10">
         <v>98</v>
       </c>
-      <c r="B10" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>MARWOOD RD</v>
-      </c>
-      <c r="G10" t="str">
-        <v>6984</v>
-      </c>
-      <c r="H10" t="str">
-        <v>F</v>
-      </c>
-      <c r="I10" t="str">
-        <v>43.25025611</v>
-      </c>
-      <c r="J10" t="str">
-        <v>-77.63379486</v>
-      </c>
-      <c r="K10" t="str">
-        <v>9302-L0247-0447-0451-ED00075</v>
-      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12">
         <v>99</v>
       </c>
-      <c r="B12" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G12" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H12" t="str">
-        <v>1</v>
-      </c>
-      <c r="I12" t="str">
-        <v>43.24243494</v>
-      </c>
-      <c r="J12" t="str">
-        <v>-77.63592396</v>
-      </c>
-      <c r="K12" t="str">
-        <v>9302-L0247-0447-0486-ED00001</v>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14">
         <v>100</v>
       </c>
-      <c r="B14" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D14" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G14" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H14" t="str">
-        <v>10</v>
-      </c>
-      <c r="I14" t="str">
-        <v>43.2458239</v>
-      </c>
-      <c r="J14" t="str">
-        <v>-77.63579026</v>
-      </c>
-      <c r="K14" t="str">
-        <v>9302-L0247-0447-0486-ED00002</v>
-      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16">
         <v>101</v>
       </c>
-      <c r="B16" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D16" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G16" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H16" t="str">
-        <v>11</v>
-      </c>
-      <c r="I16" t="str">
-        <v>43.24618343</v>
-      </c>
-      <c r="J16" t="str">
-        <v>-77.63578453</v>
-      </c>
-      <c r="K16" t="str">
-        <v>9302-L0247-0447-0486-ED00003</v>
-      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18">
         <v>102</v>
       </c>
-      <c r="B18" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D18" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G18" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H18" t="str">
-        <v>12</v>
-      </c>
-      <c r="I18" t="str">
-        <v>43.24656065</v>
-      </c>
-      <c r="J18" t="str">
-        <v>-77.63577946</v>
-      </c>
-      <c r="K18" t="str">
-        <v>9302-L0247-0447-0486-ED00004</v>
-      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20">
         <v>103</v>
       </c>
-      <c r="B20" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D20" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G20" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H20" t="str">
-        <v>13</v>
-      </c>
-      <c r="I20" t="str">
-        <v>43.24696173</v>
-      </c>
-      <c r="J20" t="str">
-        <v>-77.63578897</v>
-      </c>
-      <c r="K20" t="str">
-        <v>9302-L0247-0447-0486-ED00005</v>
-      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
     <row r="22">
       <c r="A22">
         <v>104</v>
       </c>
-      <c r="B22" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D22" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G22" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H22" t="str">
-        <v>14</v>
-      </c>
-      <c r="I22" t="str">
-        <v>43.2473541</v>
-      </c>
-      <c r="J22" t="str">
-        <v>-77.6358182</v>
-      </c>
-      <c r="K22" t="str">
-        <v>9302-L0247-0447-0486-ED00006</v>
-      </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24">
         <v>105</v>
       </c>
-      <c r="B24" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D24" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G24" t="str">
-        <v>445</v>
-      </c>
-      <c r="H24" t="str">
-        <v>2</v>
-      </c>
-      <c r="I24" t="str">
-        <v>43.24294112</v>
-      </c>
-      <c r="J24" t="str">
-        <v>-77.63595685</v>
-      </c>
-      <c r="K24" t="str">
-        <v>9302-L0247-0447-0486-ED00009</v>
-      </c>
     </row>
     <row r="25"/>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26">
         <v>106</v>
       </c>
-      <c r="B26" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D26" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G26" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H26" t="str">
-        <v>3</v>
-      </c>
-      <c r="I26" t="str">
-        <v>43.24329629</v>
-      </c>
-      <c r="J26" t="str">
-        <v>-77.63592801</v>
-      </c>
-      <c r="K26" t="str">
-        <v>9302-L0247-0447-0486-ED00010</v>
-      </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28">
         <v>107</v>
       </c>
-      <c r="B28" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D28" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G28" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H28" t="str">
-        <v>4</v>
-      </c>
-      <c r="I28" t="str">
-        <v>43.24368313</v>
-      </c>
-      <c r="J28" t="str">
-        <v>-77.63594254</v>
-      </c>
-      <c r="K28" t="str">
-        <v>9302-L0247-0447-0486-ED00011</v>
-      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30">
         <v>108</v>
       </c>
-      <c r="B30" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D30" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G30" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H30" t="str">
-        <v>5</v>
-      </c>
-      <c r="I30" t="str">
-        <v>43.24407111</v>
-      </c>
-      <c r="J30" t="str">
-        <v>-77.63593814</v>
-      </c>
-      <c r="K30" t="str">
-        <v>9302-L0247-0447-0486-ED00012</v>
-      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
     <row r="32">
       <c r="A32">
         <v>109</v>
       </c>
-      <c r="B32" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D32" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G32" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H32" t="str">
-        <v>6</v>
-      </c>
-      <c r="I32" t="str">
-        <v>43.24446141</v>
-      </c>
-      <c r="J32" t="str">
-        <v>-77.63592234</v>
-      </c>
-      <c r="K32" t="str">
-        <v>9302-L0247-0447-0486-ED00013</v>
-      </c>
     </row>
     <row r="33"/>
     <row r="34">
       <c r="A34">
         <v>110</v>
       </c>
-      <c r="B34" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D34" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G34" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H34" t="str">
-        <v>7</v>
-      </c>
-      <c r="I34" t="str">
-        <v>43.24484979</v>
-      </c>
-      <c r="J34" t="str">
-        <v>-77.63591457</v>
-      </c>
-      <c r="K34" t="str">
-        <v>9302-L0247-0447-0486-ED00014</v>
-      </c>
     </row>
     <row r="35"/>
     <row r="36">
       <c r="A36">
         <v>111</v>
       </c>
-      <c r="B36" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D36" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G36" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H36" t="str">
-        <v>8</v>
-      </c>
-      <c r="I36" t="str">
-        <v>43.2452683</v>
-      </c>
-      <c r="J36" t="str">
-        <v>-77.63592877</v>
-      </c>
-      <c r="K36" t="str">
-        <v>9302-L0247-0447-0486-ED00015</v>
-      </c>
     </row>
     <row r="37"/>
     <row r="38">
       <c r="A38">
         <v>112</v>
       </c>
-      <c r="B38" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D38" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G38" t="str">
-        <v>445</v>
-      </c>
-      <c r="H38" t="str">
-        <v>A</v>
-      </c>
-      <c r="I38" t="str">
-        <v>43.24581942</v>
-      </c>
-      <c r="J38" t="str">
-        <v>-77.63647995</v>
-      </c>
-      <c r="K38" t="str">
-        <v>9302-L0247-0447-0486-ED00016</v>
-      </c>
     </row>
     <row r="39"/>
     <row r="40">
       <c r="A40">
         <v>113</v>
       </c>
-      <c r="B40" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D40" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G40" t="str">
-        <v>445</v>
-      </c>
-      <c r="H40" t="str">
-        <v>A</v>
-      </c>
-      <c r="I40" t="str">
-        <v>43.24259681</v>
-      </c>
-      <c r="J40" t="str">
-        <v>-77.63653133</v>
-      </c>
-      <c r="K40" t="str">
-        <v>9302-L0247-0447-0486-ED00017</v>
-      </c>
     </row>
     <row r="41"/>
     <row r="42">
       <c r="A42">
         <v>114</v>
       </c>
-      <c r="B42" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D42" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G42" t="str">
-        <v>445</v>
-      </c>
-      <c r="H42" t="str">
-        <v>B</v>
-      </c>
-      <c r="I42" t="str">
-        <v>43.24293261</v>
-      </c>
-      <c r="J42" t="str">
-        <v>-77.63648662</v>
-      </c>
-      <c r="K42" t="str">
-        <v>9302-L0247-0447-0486-ED00019</v>
-      </c>
     </row>
     <row r="43"/>
     <row r="44">
       <c r="A44">
         <v>115</v>
-      </c>
-      <c r="B44" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D44" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G44" t="str">
-        <v>445</v>
-      </c>
-      <c r="H44" t="str">
-        <v>B</v>
-      </c>
-      <c r="I44" t="str">
-        <v>43.24619993</v>
-      </c>
-      <c r="J44" t="str">
-        <v>-77.63649266</v>
-      </c>
-      <c r="K44" t="str">
-        <v>9302-L0247-0447-0486-ED00020</v>
       </c>
     </row>
     <row r="45"/>
@@ -7739,296 +7361,65 @@
       <c r="A6">
         <v>116</v>
       </c>
-      <c r="B6" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D6" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G6" t="str">
-        <v>445</v>
-      </c>
-      <c r="H6" t="str">
-        <v>C</v>
-      </c>
-      <c r="I6" t="str">
-        <v>43.24658644</v>
-      </c>
-      <c r="J6" t="str">
-        <v>-77.63652933</v>
-      </c>
-      <c r="K6" t="str">
-        <v>9302-L0247-0447-0486-ED00021</v>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8">
         <v>117</v>
       </c>
-      <c r="B8" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G8" t="str">
-        <v>445</v>
-      </c>
-      <c r="H8" t="str">
-        <v>C</v>
-      </c>
-      <c r="I8" t="str">
-        <v>43.24330945</v>
-      </c>
-      <c r="J8" t="str">
-        <v>-77.63649519</v>
-      </c>
-      <c r="K8" t="str">
-        <v>9302-L0247-0447-0486-ED00022</v>
-      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10">
         <v>118</v>
       </c>
-      <c r="B10" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G10" t="str">
-        <v>445</v>
-      </c>
-      <c r="H10" t="str">
-        <v>D</v>
-      </c>
-      <c r="I10" t="str">
-        <v>43.24369909</v>
-      </c>
-      <c r="J10" t="str">
-        <v>-77.6365097</v>
-      </c>
-      <c r="K10" t="str">
-        <v>9302-L0247-0447-0486-ED00023</v>
-      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12">
         <v>119</v>
       </c>
-      <c r="B12" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G12" t="str">
-        <v>445</v>
-      </c>
-      <c r="H12" t="str">
-        <v>D</v>
-      </c>
-      <c r="I12" t="str">
-        <v>43.24695473</v>
-      </c>
-      <c r="J12" t="str">
-        <v>-77.63659514</v>
-      </c>
-      <c r="K12" t="str">
-        <v>9302-L0247-0447-0486-ED00024</v>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14">
         <v>120</v>
       </c>
-      <c r="B14" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D14" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G14" t="str">
-        <v>445</v>
-      </c>
-      <c r="H14" t="str">
-        <v>E</v>
-      </c>
-      <c r="I14" t="str">
-        <v>43.24737175</v>
-      </c>
-      <c r="J14" t="str">
-        <v>-77.63636035</v>
-      </c>
-      <c r="K14" t="str">
-        <v>9302-L0247-0447-0486-ED00025</v>
-      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16">
         <v>121</v>
       </c>
-      <c r="B16" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D16" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G16" t="str">
-        <v>445</v>
-      </c>
-      <c r="H16" t="str">
-        <v>E</v>
-      </c>
-      <c r="I16" t="str">
-        <v>43.24412096</v>
-      </c>
-      <c r="J16" t="str">
-        <v>-77.63650601</v>
-      </c>
-      <c r="K16" t="str">
-        <v>9302-L0247-0447-0486-ED00026</v>
-      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18">
         <v>122</v>
       </c>
-      <c r="B18" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D18" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G18" t="str">
-        <v>445</v>
-      </c>
-      <c r="H18" t="str">
-        <v>F</v>
-      </c>
-      <c r="I18" t="str">
-        <v>43.24446869</v>
-      </c>
-      <c r="J18" t="str">
-        <v>-77.63650779</v>
-      </c>
-      <c r="K18" t="str">
-        <v>9302-L0247-0447-0486-ED00027</v>
-      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20">
         <v>123</v>
       </c>
-      <c r="B20" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D20" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G20" t="str">
-        <v>445</v>
-      </c>
-      <c r="H20" t="str">
-        <v>G</v>
-      </c>
-      <c r="I20" t="str">
-        <v>43.24487621</v>
-      </c>
-      <c r="J20" t="str">
-        <v>-77.63649498</v>
-      </c>
-      <c r="K20" t="str">
-        <v>9302-L0247-0447-0486-ED00028</v>
-      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
     <row r="22">
       <c r="A22">
         <v>124</v>
       </c>
-      <c r="B22" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D22" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G22" t="str">
-        <v>445</v>
-      </c>
-      <c r="H22" t="str">
-        <v>H</v>
-      </c>
-      <c r="I22" t="str">
-        <v>43.24523147</v>
-      </c>
-      <c r="J22" t="str">
-        <v>-77.63645057</v>
-      </c>
-      <c r="K22" t="str">
-        <v>9302-L0247-0447-0486-ED00029</v>
-      </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24">
         <v>125</v>
       </c>
-      <c r="B24" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D24" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G24" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H24" t="str">
-        <v>2098.01</v>
-      </c>
-      <c r="I24" t="str">
-        <v>43.24197866</v>
-      </c>
-      <c r="J24" t="str">
-        <v>-77.6357927</v>
-      </c>
-      <c r="K24" t="str">
-        <v>9302-L0247-0447-0486-HH00001</v>
-      </c>
     </row>
     <row r="25"/>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26">
         <v>126</v>
-      </c>
-      <c r="B26" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D26" t="str">
-        <v>MORROW DR</v>
-      </c>
-      <c r="G26" t="str">
-        <v>7445</v>
-      </c>
-      <c r="H26" t="str">
-        <v>2098.03</v>
-      </c>
-      <c r="I26" t="str">
-        <v>43.2425355</v>
-      </c>
-      <c r="J26" t="str">
-        <v>-77.63580591</v>
-      </c>
-      <c r="K26" t="str">
-        <v>9302-L0247-0447-0486-HH00002</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
add poles amount to sheet, disable button when 1-150 poles not selected
</commit_message>
<xml_diff>
--- a/server/xlsx/od313.xlsx
+++ b/server/xlsx/od313.xlsx
@@ -746,6 +746,9 @@
       <c r="T6" t="str">
         <v>4) No. of Poles</v>
       </c>
+      <c r="X6" t="str">
+        <v>49</v>
+      </c>
       <c r="AD6" t="str">
         <v>15) Prepared By</v>
       </c>
@@ -3493,161 +3496,35 @@
       <c r="A34">
         <v>50</v>
       </c>
-      <c r="B34" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D34" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G34" t="str">
-        <v>916</v>
-      </c>
-      <c r="H34" t="str">
-        <v>12</v>
-      </c>
-      <c r="I34" t="str">
-        <v>43.25036168</v>
-      </c>
-      <c r="J34" t="str">
-        <v>-77.63177493</v>
-      </c>
-      <c r="K34" t="str">
-        <v>9302-L0089-0447-0070-ED00004</v>
-      </c>
     </row>
     <row r="35"/>
     <row r="36">
       <c r="A36">
         <v>51</v>
       </c>
-      <c r="B36" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D36" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G36" t="str">
-        <v>916</v>
-      </c>
-      <c r="H36" t="str">
-        <v>11</v>
-      </c>
-      <c r="I36" t="str">
-        <v>43.24940519</v>
-      </c>
-      <c r="J36" t="str">
-        <v>-77.63182659</v>
-      </c>
-      <c r="K36" t="str">
-        <v>9302-L0247-0447-0070-ED00003</v>
-      </c>
     </row>
     <row r="37"/>
     <row r="38">
       <c r="A38">
         <v>52</v>
       </c>
-      <c r="B38" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D38" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G38" t="str">
-        <v>916</v>
-      </c>
-      <c r="H38" t="str">
-        <v>A</v>
-      </c>
-      <c r="I38" t="str">
-        <v>43.24572959</v>
-      </c>
-      <c r="J38" t="str">
-        <v>-77.63268165</v>
-      </c>
-      <c r="K38" t="str">
-        <v>9302-L0247-0447-0070-ED00017</v>
-      </c>
     </row>
     <row r="39"/>
     <row r="40">
       <c r="A40">
         <v>53</v>
       </c>
-      <c r="B40" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D40" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G40" t="str">
-        <v>916</v>
-      </c>
-      <c r="H40" t="str">
-        <v>B</v>
-      </c>
-      <c r="I40" t="str">
-        <v>43.24591841</v>
-      </c>
-      <c r="J40" t="str">
-        <v>-77.63266817</v>
-      </c>
-      <c r="K40" t="str">
-        <v>9302-L0247-0447-0070-ED00018</v>
-      </c>
     </row>
     <row r="41"/>
     <row r="42">
       <c r="A42">
         <v>54</v>
       </c>
-      <c r="B42" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D42" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G42" t="str">
-        <v>916</v>
-      </c>
-      <c r="H42" t="str">
-        <v>C</v>
-      </c>
-      <c r="I42" t="str">
-        <v>43.24633213</v>
-      </c>
-      <c r="J42" t="str">
-        <v>-77.63263308</v>
-      </c>
-      <c r="K42" t="str">
-        <v>9302-L0247-0447-0070-ED00019</v>
-      </c>
     </row>
     <row r="43"/>
     <row r="44">
       <c r="A44">
         <v>55</v>
-      </c>
-      <c r="B44" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D44" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G44" t="str">
-        <v>916</v>
-      </c>
-      <c r="H44" t="str">
-        <v>D</v>
-      </c>
-      <c r="I44" t="str">
-        <v>43.24672723</v>
-      </c>
-      <c r="J44" t="str">
-        <v>-77.63262647</v>
-      </c>
-      <c r="K44" t="str">
-        <v>9302-L0247-0447-0070-ED00020</v>
       </c>
     </row>
     <row r="45"/>
@@ -4271,539 +4148,119 @@
       <c r="A6">
         <v>56</v>
       </c>
-      <c r="B6" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D6" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G6" t="str">
-        <v>916</v>
-      </c>
-      <c r="H6" t="str">
-        <v>E</v>
-      </c>
-      <c r="I6" t="str">
-        <v>43.24716135</v>
-      </c>
-      <c r="J6" t="str">
-        <v>-77.63262878</v>
-      </c>
-      <c r="K6" t="str">
-        <v>9302-L0247-0447-0070-ED00021</v>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8">
         <v>57</v>
       </c>
-      <c r="B8" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G8" t="str">
-        <v>916</v>
-      </c>
-      <c r="H8" t="str">
-        <v>F</v>
-      </c>
-      <c r="I8" t="str">
-        <v>43.24755135</v>
-      </c>
-      <c r="J8" t="str">
-        <v>-77.6325858</v>
-      </c>
-      <c r="K8" t="str">
-        <v>9302-L0247-0447-0070-ED00022</v>
-      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10">
         <v>58</v>
       </c>
-      <c r="B10" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G10" t="str">
-        <v>916</v>
-      </c>
-      <c r="H10" t="str">
-        <v>G</v>
-      </c>
-      <c r="I10" t="str">
-        <v>43.24796897</v>
-      </c>
-      <c r="J10" t="str">
-        <v>-77.6325781</v>
-      </c>
-      <c r="K10" t="str">
-        <v>9302-L0247-0447-0070-ED00023</v>
-      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12">
         <v>59</v>
       </c>
-      <c r="B12" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G12" t="str">
-        <v>916</v>
-      </c>
-      <c r="H12" t="str">
-        <v>G1</v>
-      </c>
-      <c r="I12" t="str">
-        <v>43.24785988</v>
-      </c>
-      <c r="J12" t="str">
-        <v>-77.63257241</v>
-      </c>
-      <c r="K12" t="str">
-        <v>9302-L0247-0447-0070-ED00024</v>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14">
         <v>60</v>
       </c>
-      <c r="B14" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D14" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G14" t="str">
-        <v>916</v>
-      </c>
-      <c r="H14" t="str">
-        <v>H</v>
-      </c>
-      <c r="I14" t="str">
-        <v>43.24837505</v>
-      </c>
-      <c r="J14" t="str">
-        <v>-77.63255257</v>
-      </c>
-      <c r="K14" t="str">
-        <v>9302-L0247-0447-0070-ED00025</v>
-      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16">
         <v>61</v>
       </c>
-      <c r="B16" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D16" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G16" t="str">
-        <v>916</v>
-      </c>
-      <c r="H16" t="str">
-        <v>J</v>
-      </c>
-      <c r="I16" t="str">
-        <v>43.24878905</v>
-      </c>
-      <c r="J16" t="str">
-        <v>-77.63260099</v>
-      </c>
-      <c r="K16" t="str">
-        <v>9302-L0247-0447-0070-ED00026</v>
-      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18">
         <v>62</v>
       </c>
-      <c r="B18" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D18" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G18" t="str">
-        <v>916</v>
-      </c>
-      <c r="H18" t="str">
-        <v>K</v>
-      </c>
-      <c r="I18" t="str">
-        <v>43.24942248</v>
-      </c>
-      <c r="J18" t="str">
-        <v>-77.63276404</v>
-      </c>
-      <c r="K18" t="str">
-        <v>9302-L0247-0447-0070-ED00027</v>
-      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20">
         <v>63</v>
       </c>
-      <c r="B20" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D20" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G20" t="str">
-        <v>916</v>
-      </c>
-      <c r="H20" t="str">
-        <v>L</v>
-      </c>
-      <c r="I20" t="str">
-        <v>43.24941445</v>
-      </c>
-      <c r="J20" t="str">
-        <v>-77.63217786</v>
-      </c>
-      <c r="K20" t="str">
-        <v>9302-L0247-0447-0070-ED00028</v>
-      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
     <row r="22">
       <c r="A22">
         <v>64</v>
       </c>
-      <c r="B22" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D22" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G22" t="str">
-        <v>916</v>
-      </c>
-      <c r="H22" t="str">
-        <v>M</v>
-      </c>
-      <c r="I22" t="str">
-        <v>43.24919993</v>
-      </c>
-      <c r="J22" t="str">
-        <v>-77.63251813</v>
-      </c>
-      <c r="K22" t="str">
-        <v>9302-L0247-0447-0070-ED00029</v>
-      </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24">
         <v>65</v>
       </c>
-      <c r="B24" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D24" t="str">
-        <v>BISCAYNE DR</v>
-      </c>
-      <c r="G24" t="str">
-        <v>916</v>
-      </c>
-      <c r="H24" t="str">
-        <v>N</v>
-      </c>
-      <c r="I24" t="str">
-        <v>43.24940865</v>
-      </c>
-      <c r="J24" t="str">
-        <v>-77.63251207</v>
-      </c>
-      <c r="K24" t="str">
-        <v>9302-L0247-0447-0070-ED00030</v>
-      </c>
     </row>
     <row r="25"/>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26">
         <v>66</v>
       </c>
-      <c r="B26" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D26" t="str">
-        <v>GREENLEAF RD</v>
-      </c>
-      <c r="G26" t="str">
-        <v>4608</v>
-      </c>
-      <c r="H26" t="str">
-        <v>1</v>
-      </c>
-      <c r="I26" t="str">
-        <v>43.25294659</v>
-      </c>
-      <c r="J26" t="str">
-        <v>-77.62829745</v>
-      </c>
-      <c r="K26" t="str">
-        <v>9302-L0089-0447-0298-ED00008</v>
-      </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28">
         <v>67</v>
       </c>
-      <c r="B28" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D28" t="str">
-        <v>GREENLEAF RD</v>
-      </c>
-      <c r="G28" t="str">
-        <v>4608</v>
-      </c>
-      <c r="H28" t="str">
-        <v>3</v>
-      </c>
-      <c r="I28" t="str">
-        <v>43.25353813</v>
-      </c>
-      <c r="J28" t="str">
-        <v>-77.62826796</v>
-      </c>
-      <c r="K28" t="str">
-        <v>9302-L0089-0447-0298-ED00031</v>
-      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30">
         <v>68</v>
       </c>
-      <c r="B30" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D30" t="str">
-        <v>GREENLEAF RD</v>
-      </c>
-      <c r="G30" t="str">
-        <v>4608</v>
-      </c>
-      <c r="H30" t="str">
-        <v>2</v>
-      </c>
-      <c r="I30" t="str">
-        <v>43.25328475</v>
-      </c>
-      <c r="J30" t="str">
-        <v>-77.62825755</v>
-      </c>
-      <c r="K30" t="str">
-        <v>9302-L0089-0447-0298-ED00044</v>
-      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
     <row r="32">
       <c r="A32">
         <v>69</v>
       </c>
-      <c r="B32" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D32" t="str">
-        <v>GREENLEAF RD</v>
-      </c>
-      <c r="G32" t="str">
-        <v>4608</v>
-      </c>
-      <c r="H32" t="str">
-        <v>1848.01</v>
-      </c>
-      <c r="I32" t="str">
-        <v>43.25337478</v>
-      </c>
-      <c r="J32" t="str">
-        <v>-77.62835434</v>
-      </c>
-      <c r="K32" t="str">
-        <v>9302-L0355-0447-0298-MH00101</v>
-      </c>
     </row>
     <row r="33"/>
     <row r="34">
       <c r="A34">
         <v>70</v>
       </c>
-      <c r="B34" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D34" t="str">
-        <v>CLEARVIEW RD</v>
-      </c>
-      <c r="G34" t="str">
-        <v>2144</v>
-      </c>
-      <c r="H34" t="str">
-        <v>8</v>
-      </c>
-      <c r="I34" t="str">
-        <v>43.24163412</v>
-      </c>
-      <c r="J34" t="str">
-        <v>-77.62954065</v>
-      </c>
-      <c r="K34" t="str">
-        <v>9302-L0247-0447-0136-ED00011</v>
-      </c>
     </row>
     <row r="35"/>
     <row r="36">
       <c r="A36">
         <v>71</v>
       </c>
-      <c r="B36" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D36" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G36" t="str">
-        <v>192</v>
-      </c>
-      <c r="H36" t="str">
-        <v>11C</v>
-      </c>
-      <c r="I36" t="str">
-        <v>43.24250539</v>
-      </c>
-      <c r="J36" t="str">
-        <v>-77.64494276</v>
-      </c>
-      <c r="K36" t="str">
-        <v>9302-L0247-0447-0406-ED00005</v>
-      </c>
     </row>
     <row r="37"/>
     <row r="38">
       <c r="A38">
         <v>72</v>
       </c>
-      <c r="B38" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D38" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G38" t="str">
-        <v>192</v>
-      </c>
-      <c r="H38" t="str">
-        <v>11D</v>
-      </c>
-      <c r="I38" t="str">
-        <v>43.24247634</v>
-      </c>
-      <c r="J38" t="str">
-        <v>-77.64450783</v>
-      </c>
-      <c r="K38" t="str">
-        <v>9302-L0247-0447-0406-ED00006</v>
-      </c>
     </row>
     <row r="39"/>
     <row r="40">
       <c r="A40">
         <v>73</v>
       </c>
-      <c r="B40" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D40" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G40" t="str">
-        <v>192</v>
-      </c>
-      <c r="H40" t="str">
-        <v>11E</v>
-      </c>
-      <c r="I40" t="str">
-        <v>43.24250994</v>
-      </c>
-      <c r="J40" t="str">
-        <v>-77.64417309</v>
-      </c>
-      <c r="K40" t="str">
-        <v>9302-L0247-0447-0406-ED00007</v>
-      </c>
     </row>
     <row r="41"/>
     <row r="42">
       <c r="A42">
         <v>74</v>
       </c>
-      <c r="B42" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D42" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G42" t="str">
-        <v>192</v>
-      </c>
-      <c r="H42" t="str">
-        <v>11F</v>
-      </c>
-      <c r="I42" t="str">
-        <v>43.24216425</v>
-      </c>
-      <c r="J42" t="str">
-        <v>-77.64609089</v>
-      </c>
-      <c r="K42" t="str">
-        <v>9302-L0248-0447-0406-ED00008</v>
-      </c>
     </row>
     <row r="43"/>
     <row r="44">
       <c r="A44">
         <v>75</v>
-      </c>
-      <c r="B44" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D44" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G44" t="str">
-        <v>192</v>
-      </c>
-      <c r="H44" t="str">
-        <v>11G</v>
-      </c>
-      <c r="I44" t="str">
-        <v>43.24252223</v>
-      </c>
-      <c r="J44" t="str">
-        <v>-77.6461087</v>
-      </c>
-      <c r="K44" t="str">
-        <v>9302-L0248-0447-0406-ED00009</v>
       </c>
     </row>
     <row r="45"/>
@@ -5427,539 +4884,119 @@
       <c r="A6">
         <v>76</v>
       </c>
-      <c r="B6" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D6" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G6" t="str">
-        <v>192</v>
-      </c>
-      <c r="H6" t="str">
-        <v>1</v>
-      </c>
-      <c r="I6" t="str">
-        <v>43.2439159</v>
-      </c>
-      <c r="J6" t="str">
-        <v>-77.64663618</v>
-      </c>
-      <c r="K6" t="str">
-        <v>9302-L0250-0447-0406-ED00001</v>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8">
         <v>77</v>
       </c>
-      <c r="B8" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G8" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H8" t="str">
-        <v>11A</v>
-      </c>
-      <c r="I8" t="str">
-        <v>43.24355134</v>
-      </c>
-      <c r="J8" t="str">
-        <v>-77.64614036</v>
-      </c>
-      <c r="K8" t="str">
-        <v>9302-L0250-0447-0406-ED00003</v>
-      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10">
         <v>78</v>
       </c>
-      <c r="B10" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G10" t="str">
-        <v>192</v>
-      </c>
-      <c r="H10" t="str">
-        <v>11B</v>
-      </c>
-      <c r="I10" t="str">
-        <v>43.24309891</v>
-      </c>
-      <c r="J10" t="str">
-        <v>-77.64614836</v>
-      </c>
-      <c r="K10" t="str">
-        <v>9302-L0250-0447-0406-ED00004</v>
-      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1"/>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12">
         <v>79</v>
       </c>
-      <c r="B12" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D12" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G12" t="str">
-        <v>192</v>
-      </c>
-      <c r="H12" t="str">
-        <v>11H</v>
-      </c>
-      <c r="I12" t="str">
-        <v>43.24328515</v>
-      </c>
-      <c r="J12" t="str">
-        <v>-77.64504899</v>
-      </c>
-      <c r="K12" t="str">
-        <v>9302-L0250-0447-0406-ED00010</v>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1"/>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14">
         <v>80</v>
       </c>
-      <c r="B14" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D14" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G14" t="str">
-        <v>192</v>
-      </c>
-      <c r="H14" t="str">
-        <v>11J</v>
-      </c>
-      <c r="I14" t="str">
-        <v>43.24333866</v>
-      </c>
-      <c r="J14" t="str">
-        <v>-77.64443704</v>
-      </c>
-      <c r="K14" t="str">
-        <v>9302-L0250-0447-0406-ED00011</v>
-      </c>
     </row>
     <row r="15" ht="12.75" customHeight="1"/>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16">
         <v>81</v>
       </c>
-      <c r="B16" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D16" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G16" t="str">
-        <v>192</v>
-      </c>
-      <c r="H16" t="str">
-        <v>11K</v>
-      </c>
-      <c r="I16" t="str">
-        <v>43.24335649</v>
-      </c>
-      <c r="J16" t="str">
-        <v>-77.64416206</v>
-      </c>
-      <c r="K16" t="str">
-        <v>9302-L0250-0447-0406-ED00012</v>
-      </c>
     </row>
     <row r="17" ht="12.75" customHeight="1"/>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18">
         <v>82</v>
       </c>
-      <c r="B18" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D18" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G18" t="str">
-        <v>192</v>
-      </c>
-      <c r="H18" t="str">
-        <v>11L</v>
-      </c>
-      <c r="I18" t="str">
-        <v>43.24352172</v>
-      </c>
-      <c r="J18" t="str">
-        <v>-77.6436245</v>
-      </c>
-      <c r="K18" t="str">
-        <v>9302-L0250-0447-0406-ED00013</v>
-      </c>
     </row>
     <row r="19" ht="12.75" customHeight="1"/>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20">
         <v>83</v>
       </c>
-      <c r="B20" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D20" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G20" t="str">
-        <v>192</v>
-      </c>
-      <c r="H20" t="str">
-        <v>11M1</v>
-      </c>
-      <c r="I20" t="str">
-        <v>43.24368718</v>
-      </c>
-      <c r="J20" t="str">
-        <v>-77.64286205</v>
-      </c>
-      <c r="K20" t="str">
-        <v>9302-L0250-0447-0406-ED00014</v>
-      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1"/>
     <row r="22">
       <c r="A22">
         <v>84</v>
       </c>
-      <c r="B22" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D22" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G22" t="str">
-        <v>192</v>
-      </c>
-      <c r="H22" t="str">
-        <v>11N</v>
-      </c>
-      <c r="I22" t="str">
-        <v>43.24398278</v>
-      </c>
-      <c r="J22" t="str">
-        <v>-77.64267074</v>
-      </c>
-      <c r="K22" t="str">
-        <v>9302-L0250-0447-0406-ED00015</v>
-      </c>
     </row>
     <row r="23"/>
     <row r="24">
       <c r="A24">
         <v>85</v>
       </c>
-      <c r="B24" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D24" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G24" t="str">
-        <v>192</v>
-      </c>
-      <c r="H24" t="str">
-        <v>11O</v>
-      </c>
-      <c r="I24" t="str">
-        <v>43.24421886</v>
-      </c>
-      <c r="J24" t="str">
-        <v>-77.6423789</v>
-      </c>
-      <c r="K24" t="str">
-        <v>9302-L0250-0447-0406-ED00016</v>
-      </c>
     </row>
     <row r="25"/>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26">
         <v>86</v>
       </c>
-      <c r="B26" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D26" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G26" t="str">
-        <v>192</v>
-      </c>
-      <c r="H26" t="str">
-        <v>11P</v>
-      </c>
-      <c r="I26" t="str">
-        <v>43.24456409</v>
-      </c>
-      <c r="J26" t="str">
-        <v>-77.6419979</v>
-      </c>
-      <c r="K26" t="str">
-        <v>9302-L0250-0447-0406-ED00017</v>
-      </c>
     </row>
     <row r="27" ht="12.75" customHeight="1"/>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28">
         <v>87</v>
       </c>
-      <c r="B28" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D28" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G28" t="str">
-        <v>192</v>
-      </c>
-      <c r="H28" t="str">
-        <v>11Q</v>
-      </c>
-      <c r="I28" t="str">
-        <v>43.2447372</v>
-      </c>
-      <c r="J28" t="str">
-        <v>-77.64181454</v>
-      </c>
-      <c r="K28" t="str">
-        <v>9302-L0250-0447-0406-ED00018</v>
-      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1"/>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30">
         <v>88</v>
       </c>
-      <c r="B30" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D30" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G30" t="str">
-        <v>192</v>
-      </c>
-      <c r="H30" t="str">
-        <v>11R</v>
-      </c>
-      <c r="I30" t="str">
-        <v>43.24404953</v>
-      </c>
-      <c r="J30" t="str">
-        <v>-77.64227728</v>
-      </c>
-      <c r="K30" t="str">
-        <v>9302-L0250-0447-0406-ED00019</v>
-      </c>
     </row>
     <row r="31" ht="12.75" customHeight="1"/>
     <row r="32">
       <c r="A32">
         <v>89</v>
       </c>
-      <c r="B32" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D32" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G32" t="str">
-        <v>192</v>
-      </c>
-      <c r="H32" t="str">
-        <v>11S</v>
-      </c>
-      <c r="I32" t="str">
-        <v>43.24360381</v>
-      </c>
-      <c r="J32" t="str">
-        <v>-77.64227764</v>
-      </c>
-      <c r="K32" t="str">
-        <v>9302-L0250-0447-0406-ED00020</v>
-      </c>
     </row>
     <row r="33"/>
     <row r="34">
       <c r="A34">
         <v>90</v>
       </c>
-      <c r="B34" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D34" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G34" t="str">
-        <v>192</v>
-      </c>
-      <c r="H34" t="str">
-        <v>11T</v>
-      </c>
-      <c r="I34" t="str">
-        <v>43.24312364</v>
-      </c>
-      <c r="J34" t="str">
-        <v>-77.64408081</v>
-      </c>
-      <c r="K34" t="str">
-        <v>9302-L0250-0447-0406-ED00021</v>
-      </c>
     </row>
     <row r="35"/>
     <row r="36">
       <c r="A36">
         <v>91</v>
       </c>
-      <c r="B36" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D36" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G36" t="str">
-        <v>192</v>
-      </c>
-      <c r="H36" t="str">
-        <v>11U</v>
-      </c>
-      <c r="I36" t="str">
-        <v>43.24290411</v>
-      </c>
-      <c r="J36" t="str">
-        <v>-77.64424673</v>
-      </c>
-      <c r="K36" t="str">
-        <v>9302-L0250-0447-0406-ED00022</v>
-      </c>
     </row>
     <row r="37"/>
     <row r="38">
       <c r="A38">
         <v>92</v>
       </c>
-      <c r="B38" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D38" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G38" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H38" t="str">
-        <v>11V</v>
-      </c>
-      <c r="I38" t="str">
-        <v>43.24327431</v>
-      </c>
-      <c r="J38" t="str">
-        <v>-77.6453732</v>
-      </c>
-      <c r="K38" t="str">
-        <v>9302-L0250-0447-0406-ED00023</v>
-      </c>
     </row>
     <row r="39"/>
     <row r="40">
       <c r="A40">
         <v>93</v>
       </c>
-      <c r="B40" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D40" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G40" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H40" t="str">
-        <v>2</v>
-      </c>
-      <c r="I40" t="str">
-        <v>43.24390094</v>
-      </c>
-      <c r="J40" t="str">
-        <v>-77.64613418</v>
-      </c>
-      <c r="K40" t="str">
-        <v>9302-L0250-0447-0406-ED00024</v>
-      </c>
     </row>
     <row r="41"/>
     <row r="42">
       <c r="A42">
         <v>94</v>
       </c>
-      <c r="B42" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D42" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G42" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H42" t="str">
-        <v>3</v>
-      </c>
-      <c r="I42" t="str">
-        <v>43.2439094</v>
-      </c>
-      <c r="J42" t="str">
-        <v>-77.64542462</v>
-      </c>
-      <c r="K42" t="str">
-        <v>9302-L0250-0447-0406-ED00025</v>
-      </c>
     </row>
     <row r="43"/>
     <row r="44">
       <c r="A44">
         <v>95</v>
-      </c>
-      <c r="B44" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D44" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G44" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H44" t="str">
-        <v>4</v>
-      </c>
-      <c r="I44" t="str">
-        <v>43.24389429</v>
-      </c>
-      <c r="J44" t="str">
-        <v>-77.64493783</v>
-      </c>
-      <c r="K44" t="str">
-        <v>9302-L0250-0447-0406-ED00026</v>
       </c>
     </row>
     <row r="45"/>
@@ -6583,53 +5620,11 @@
       <c r="A6">
         <v>96</v>
       </c>
-      <c r="B6" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D6" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G6" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H6" t="str">
-        <v>11M</v>
-      </c>
-      <c r="I6" t="str">
-        <v>43.24375654</v>
-      </c>
-      <c r="J6" t="str">
-        <v>-77.64315943</v>
-      </c>
-      <c r="K6" t="str">
-        <v>9302-L0250-0447-0406-ED00032</v>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8">
         <v>97</v>
-      </c>
-      <c r="B8" t="str">
-        <v>GREECE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>LAWSON RD</v>
-      </c>
-      <c r="G8" t="str">
-        <v>6192</v>
-      </c>
-      <c r="H8" t="str">
-        <v>2140.06</v>
-      </c>
-      <c r="I8" t="str">
-        <v>43.24387458</v>
-      </c>
-      <c r="J8" t="str">
-        <v>-77.64502817</v>
-      </c>
-      <c r="K8" t="str">
-        <v>9302-L0250-0447-0406-HH00001</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1"/>

</xml_diff>